<commit_message>
Added trend and conditional formatting in Sales by Country
</commit_message>
<xml_diff>
--- a/DataVisualization.xlsx
+++ b/DataVisualization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Synt4x\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76BAB850-4C31-4D03-96B1-C753667B14A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1CBBD2-A48F-43CB-B879-972F4899B7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A15B3FEA-B764-184D-BC44-F828B0BB3928}"/>
   </bookViews>
@@ -1976,7 +1976,7 @@
   <dimension ref="B2:AB33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2631,6 +2631,15 @@
     <mergeCell ref="J17:O17"/>
     <mergeCell ref="T16:W16"/>
   </mergeCells>
+  <conditionalFormatting sqref="H20:H25">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Flags">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V18:W18 AA18:AB18" xr:uid="{50F3DB00-790A-47C5-9D5C-6DEC891739B0}">
       <formula1>0</formula1>
@@ -2644,7 +2653,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{4F4CAF9B-E08D-4434-9FC5-12030D85085C}">
+          <x14:cfRule type="iconSet" priority="2" id="{4F4CAF9B-E08D-4434-9FC5-12030D85085C}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -2664,6 +2673,46 @@
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup lineWeight="1" displayEmptyCellsAs="gap" xr2:uid="{5815F07C-0D1E-4F31-9C7A-DCA383C090A0}">
+          <x14:colorSeries rgb="FF376092"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>Dashboard!C20:F20</xm:f>
+              <xm:sqref>G20</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Dashboard!C21:F21</xm:f>
+              <xm:sqref>G21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Dashboard!C22:F22</xm:f>
+              <xm:sqref>G22</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Dashboard!C23:F23</xm:f>
+              <xm:sqref>G23</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Dashboard!C24:F24</xm:f>
+              <xm:sqref>G24</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>Dashboard!C25:F25</xm:f>
+              <xm:sqref>G25</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
   </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added next Donut Chart
</commit_message>
<xml_diff>
--- a/DataVisualization.xlsx
+++ b/DataVisualization.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Synt4x\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Synt4x\Desktop\Data Analyst Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415A7A89-91B6-43B4-A232-F9124A49E2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6E3AB0-4F0E-45B6-92E6-BE835F42120A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A15B3FEA-B764-184D-BC44-F828B0BB3928}"/>
   </bookViews>
@@ -462,13 +462,13 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{B8BD2171-DF59-45E3-A9A6-4C72F93FBED5}"/>
@@ -950,6 +950,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F3BD-4624-B6C3-92870DF890D0}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1141,8 +1146,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.1928185262985527E-3"/>
-                  <c:y val="1.4686420634814172E-3"/>
+                  <c:x val="1.0982135722465557E-2"/>
+                  <c:y val="1.4688258498633457E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1195,7 +1200,7 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable>
                     <c15:dlblFTEntry>
-                      <c15:txfldGUID>{0C6B7250-B6DB-41F9-B9C2-9E9F62B72FE7}</c15:txfldGUID>
+                      <c15:txfldGUID>{8A6DADBF-C642-4AC3-B415-C38E2945DD84}</c15:txfldGUID>
                       <c15:f>Dashboard!$V$18</c15:f>
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
@@ -1272,6 +1277,439 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-4FD3-4B90-ABA2-8A55FC3899E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="270"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.28192299130844156"/>
+          <c:y val="6.4620250793182357E-2"/>
+          <c:w val="0.48164615097265112"/>
+          <c:h val="0.87075949841363531"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-EAD8-48F4-A821-F266EF5E43FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-EAD8-48F4-A821-F266EF5E43FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-EAD8-48F4-A821-F266EF5E43FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-EAD8-48F4-A821-F266EF5E43FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-EAD8-48F4-A821-F266EF5E43FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>Dashboard!$Z$21:$Z$25</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-EAD8-48F4-A821-F266EF5E43FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="270"/>
+        <c:holeSize val="55"/>
+      </c:doughnutChart>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dashboard!$AA$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Point</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-EAD8-48F4-A821-F266EF5E43FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-EAD8-48F4-A821-F266EF5E43FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-EAD8-48F4-A821-F266EF5E43FD}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8738983066624022E-3"/>
+                  <c:y val="1.4804694603630531E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:strRef>
+                  <c:f>Dashboard!$AA$18</c:f>
+                  <c:strCache>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>45%</c:v>
+                    </c:pt>
+                  </c:strCache>
+                </c:strRef>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{B8AE880A-0C72-43F8-B2CC-EAD789BABE76}</c15:txfldGUID>
+                      <c15:f>Dashboard!$AA$18</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>45%</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-EAD8-48F4-A821-F266EF5E43FD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Dashboard!$AA$21:$AA$23</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00%">
+                  <c:v>1.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-EAD8-48F4-A821-F266EF5E43FD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1411,6 +1849,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -1917,6 +2395,525 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2698,6 +3695,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>426008</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>184743</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>252255</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>158994</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E44CEEDF-98E3-4BB2-A009-D5A3A5A1C5E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3000,8 +4035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3B3621-7A7D-414F-AEC3-D2B91D4CBBC6}">
   <dimension ref="B2:AB33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3047,22 +4082,22 @@
       <c r="AB2" s="12"/>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
       <c r="T4" s="27" t="s">
         <v>3</v>
       </c>
@@ -3172,8 +4207,8 @@
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="T16" s="27" t="s">
@@ -3192,23 +4227,23 @@
       <c r="AB16" s="27"/>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="J17" s="26" t="s">
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="J17" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
       <c r="S17" s="8"/>
       <c r="T17" s="9"/>
       <c r="U17" s="9"/>
@@ -3525,23 +4560,23 @@
       <c r="AB27" s="27"/>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="J28" s="26" t="s">
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="J28" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
       <c r="U28" s="25" t="s">
         <v>38</v>
       </c>
@@ -3639,16 +4674,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="T16:W16"/>
     <mergeCell ref="Y16:AB16"/>
     <mergeCell ref="Y27:AB27"/>
     <mergeCell ref="T27:W27"/>
     <mergeCell ref="B4:O4"/>
     <mergeCell ref="T4:W4"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="J28:O28"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="T16:W16"/>
   </mergeCells>
   <conditionalFormatting sqref="H20:H25">
     <cfRule type="iconSet" priority="1">

</xml_diff>